<commit_message>
do not call test_local
</commit_message>
<xml_diff>
--- a/testdata/gemini/sample_gemini.xlsx
+++ b/testdata/gemini/sample_gemini.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Account History" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -448,44 +448,44 @@
   </sheetPr>
   <dimension ref="A1:AJ65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="AC36" activeCellId="0" sqref="AC36"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="20" min="16" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.9438775510204"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="24.7295918367347"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="81.6683673469388"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="43.8724489795918"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="81.6683673469388"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="43.8724489795918"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="20" min="16" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="80.7244897959184"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="80.7244897959184"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,37 +1250,25 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>43093.8942320949</v>
+        <v>43093.8948416551</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>43093.8942320949</v>
+        <v>43093.8948416551</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="10" t="n">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H15" s="4" t="n">
-        <v>5318.448</v>
-      </c>
-      <c r="I15" s="4" t="n">
-        <v>-13.29612</v>
+        <v>-5305.15</v>
       </c>
       <c r="J15" s="4" t="n">
-        <v>5305.15475028599</v>
-      </c>
-      <c r="K15" s="5" t="n">
-        <v>-0.4</v>
+        <v>0.004750285992</v>
       </c>
       <c r="M15" s="5" t="n">
         <v>0</v>
@@ -1296,38 +1284,32 @@
       </c>
       <c r="Y15" s="9" t="n">
         <v>0</v>
-      </c>
-      <c r="AB15" s="2" t="n">
-        <v>43093.8940805208</v>
-      </c>
-      <c r="AC15" s="3" t="n">
-        <v>43093.8940805208</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>43093.8948416551</v>
+        <v>43093.8991802199</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>43093.8948416551</v>
+        <v>43093.8991802199</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="4" t="n">
-        <v>-5305.15</v>
+        <v>50</v>
       </c>
       <c r="J16" s="4" t="n">
         <v>0.004750285992</v>
       </c>
+      <c r="K16" s="5" t="n">
+        <v>0.4</v>
+      </c>
       <c r="M16" s="5" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="P16" s="6" t="n">
         <v>0</v>
@@ -1339,33 +1321,48 @@
         <v>0</v>
       </c>
       <c r="Y16" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>43093.8991802199</v>
+        <v>43093.9976678935</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>43093.8991802199</v>
+        <v>43093.9976678935</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="10" t="n">
+        <v>25</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>7049.995</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <v>-17.6249875</v>
       </c>
       <c r="J17" s="4" t="n">
-        <v>0.004750285992</v>
+        <v>7032.37856278599</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>0.4</v>
+        <v>-0.5</v>
       </c>
       <c r="M17" s="5" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="P17" s="6" t="n">
         <v>0</v>
@@ -1379,16 +1376,19 @@
       <c r="Y17" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="AH17" s="11" t="n">
-        <v>0</v>
+      <c r="AB17" s="2" t="n">
+        <v>43093.9976678935</v>
+      </c>
+      <c r="AC17" s="3" t="n">
+        <v>43093.9976678935</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
-        <v>43093.9976678935</v>
+        <v>43114.1042495718</v>
       </c>
       <c r="B18" s="3" t="n">
-        <v>43093.9976678935</v>
+        <v>43114.1042495718</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>43</v>
@@ -1406,19 +1406,19 @@
         <v>25</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>7049.995</v>
+        <v>497.441</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>-17.6249875</v>
+        <v>-1.2436025</v>
       </c>
       <c r="J18" s="4" t="n">
-        <v>7032.37856278599</v>
+        <v>10107.2380497899</v>
       </c>
       <c r="K18" s="5" t="n">
-        <v>-0.5</v>
+        <v>-0.035</v>
       </c>
       <c r="M18" s="5" t="n">
-        <v>0</v>
+        <v>0.28644134</v>
       </c>
       <c r="P18" s="6" t="n">
         <v>0</v>
@@ -1433,18 +1433,18 @@
         <v>0</v>
       </c>
       <c r="AB18" s="2" t="n">
-        <v>43093.9976678935</v>
+        <v>43114.1042495718</v>
       </c>
       <c r="AC18" s="3" t="n">
-        <v>43093.9976678935</v>
+        <v>43114.1042495718</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <v>43114.1042495718</v>
+        <v>43114.1042668171</v>
       </c>
       <c r="B19" s="3" t="n">
-        <v>43114.1042495718</v>
+        <v>43114.1042668171</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>43</v>
@@ -1456,25 +1456,25 @@
         <v>41</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G19" s="10" t="n">
         <v>25</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>497.441</v>
+        <v>499.5080873726</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>-1.2436025</v>
+        <v>-1.2487702184315</v>
       </c>
       <c r="J19" s="4" t="n">
-        <v>10107.2380497899</v>
+        <v>10605.497366944</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>-0.035</v>
+        <v>-0.03518002</v>
       </c>
       <c r="M19" s="5" t="n">
-        <v>0.28644134</v>
+        <v>0.25126132</v>
       </c>
       <c r="P19" s="6" t="n">
         <v>0</v>
@@ -1497,10 +1497,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
-        <v>43114.1042668171</v>
+        <v>43114.104283588</v>
       </c>
       <c r="B20" s="3" t="n">
-        <v>43114.1042668171</v>
+        <v>43114.104283588</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>43</v>
@@ -1518,19 +1518,19 @@
         <v>25</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>499.5080873726</v>
+        <v>489.4531855518</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>-1.2487702184315</v>
+        <v>-1.2236329638795</v>
       </c>
       <c r="J20" s="4" t="n">
-        <v>10605.497366944</v>
+        <v>11093.726919532</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>-0.03518002</v>
+        <v>-0.03447186</v>
       </c>
       <c r="M20" s="5" t="n">
-        <v>0.25126132</v>
+        <v>0.21678946</v>
       </c>
       <c r="P20" s="6" t="n">
         <v>0</v>
@@ -1553,10 +1553,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
-        <v>43114.104283588</v>
+        <v>43114.1042929514</v>
       </c>
       <c r="B21" s="3" t="n">
-        <v>43114.104283588</v>
+        <v>43114.1042929514</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>43</v>
@@ -1574,19 +1574,19 @@
         <v>25</v>
       </c>
       <c r="H21" s="4" t="n">
-        <v>489.4531855518</v>
+        <v>150.1911203318</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>-1.2236329638795</v>
+        <v>-0.3754778008295</v>
       </c>
       <c r="J21" s="4" t="n">
-        <v>11093.726919532</v>
+        <v>11243.5425620629</v>
       </c>
       <c r="K21" s="5" t="n">
-        <v>-0.03447186</v>
+        <v>-0.01057786</v>
       </c>
       <c r="M21" s="5" t="n">
-        <v>0.21678946</v>
+        <v>0.2062116</v>
       </c>
       <c r="P21" s="6" t="n">
         <v>0</v>
@@ -1609,10 +1609,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
-        <v>43114.1042929514</v>
+        <v>43114.1043009259</v>
       </c>
       <c r="B22" s="3" t="n">
-        <v>43114.1042929514</v>
+        <v>43114.1043009259</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>43</v>
@@ -1630,19 +1630,19 @@
         <v>25</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>150.1911203318</v>
+        <v>496.95205</v>
       </c>
       <c r="I22" s="4" t="n">
-        <v>-0.3754778008295</v>
+        <v>-1.242380125</v>
       </c>
       <c r="J22" s="4" t="n">
-        <v>11243.5425620629</v>
+        <v>11739.2522319379</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>-0.01057786</v>
+        <v>-0.035</v>
       </c>
       <c r="M22" s="5" t="n">
-        <v>0.2062116</v>
+        <v>0.1712116</v>
       </c>
       <c r="P22" s="6" t="n">
         <v>0</v>
@@ -1663,102 +1663,47 @@
         <v>43114.1042495718</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
-        <v>43114.1043009259</v>
-      </c>
-      <c r="B23" s="3" t="n">
-        <v>43114.1043009259</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="10" t="n">
-        <v>25</v>
-      </c>
-      <c r="H23" s="4" t="n">
-        <v>496.95205</v>
-      </c>
-      <c r="I23" s="4" t="n">
-        <v>-1.242380125</v>
-      </c>
-      <c r="J23" s="4" t="n">
-        <v>11739.2522319379</v>
-      </c>
-      <c r="K23" s="5" t="n">
-        <v>-0.035</v>
-      </c>
-      <c r="M23" s="5" t="n">
-        <v>0.1712116</v>
-      </c>
-      <c r="P23" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="V23" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="2" t="n">
-        <v>43114.1042495718</v>
-      </c>
-      <c r="AC23" s="3" t="n">
-        <v>43114.1042495718</v>
-      </c>
-    </row>
-    <row r="24" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="13" t="s">
+    <row r="23" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H23" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="14" t="n">
+      <c r="I23" s="14" t="n">
         <v>-159.071846433698</v>
       </c>
-      <c r="J24" s="14" t="n">
+      <c r="J23" s="14" t="n">
         <v>0.00673189900225</v>
       </c>
-      <c r="L24" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="S24" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="U24" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="X24" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF24" s="0"/>
-      <c r="AG24" s="0"/>
-    </row>
+      <c r="L23" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="0"/>
+      <c r="AG23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1786,7 +1731,7 @@
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>